<commit_message>
updated netflix sub count
</commit_message>
<xml_diff>
--- a/Data/DataNetflixSubscriber2020_V2.xlsx
+++ b/Data/DataNetflixSubscriber2020_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25423"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3f45\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alliepanacci/Documents/GitHub/SST---Final-Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29D41198-FCA5-40DE-BBB2-E4088870EBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B5AD2B-2665-1744-851B-E5FF4A08480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -925,11 +925,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C41" sqref="A1:C41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,7 +942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -951,7 +953,7 @@
         <v>60909000</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -962,7 +964,7 @@
         <v>29339000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -973,7 +975,7 @@
         <v>21260000</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -984,7 +986,7 @@
         <v>7394000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -995,7 +997,7 @@
         <v>61870000</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1006,7 +1008,7 @@
         <v>31317000</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1019,7 @@
         <v>22795000</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1030,7 @@
         <v>8372000</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1039,7 +1041,7 @@
         <v>63010000</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1052,7 @@
         <v>33836000</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1061,7 +1063,7 @@
         <v>24115000</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1072,7 +1074,7 @@
         <v>9461000</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1083,7 +1085,7 @@
         <v>64757000</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1094,7 +1096,7 @@
         <v>37818000</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1105,7 +1107,7 @@
         <v>26077000</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1118,7 @@
         <v>10607000</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1127,7 +1129,7 @@
         <v>66633000</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1138,7 +1140,7 @@
         <v>42542000</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1149,7 +1151,7 @@
         <v>27547000</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1160,7 +1162,7 @@
         <v>12141000</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1171,7 +1173,7 @@
         <v>66501000</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1182,7 +1184,7 @@
         <v>44229000</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1193,7 +1195,7 @@
         <v>27890000</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1204,7 +1206,7 @@
         <v>12942000</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1215,7 +1217,7 @@
         <v>67114000</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1228,7 @@
         <v>47355000</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1237,7 +1239,7 @@
         <v>29380000</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1248,7 +1250,7 @@
         <v>14485000</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1261,7 @@
         <v>67662000</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1270,7 +1272,7 @@
         <v>51778000</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1281,7 +1283,7 @@
         <v>31417000</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1292,7 +1294,7 @@
         <v>16233000</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1303,7 +1305,7 @@
         <v>69969000</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1314,7 +1316,7 @@
         <v>58734000</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1325,7 +1327,7 @@
         <v>34318000</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1336,7 +1338,7 @@
         <v>19835000</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>72904000</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1358,7 +1360,7 @@
         <v>61483000</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1369,7 +1371,7 @@
         <v>36068000</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>7</v>
       </c>

</xml_diff>